<commit_message>
aggiunte tabelle periodi prog. arch.
</commit_message>
<xml_diff>
--- a/DocEsterna/PianoDiProgetto/Charts/GraficiPreventivo.xlsx
+++ b/DocEsterna/PianoDiProgetto/Charts/GraficiPreventivo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SWE\RepoDocumentazione\CodeBusters-Docs\Doc_esterna\PianoDiProgetto\Charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SWE\RepoDocumentazione\CodeBusters-Docs\DocEsterna\PianoDiProgetto\Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F7AFF3-3942-495A-92E8-0C29535A4387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EF0315-0895-45B0-B86B-2DBB712070AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17040" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="26">
   <si>
     <t>Baldisseri Michele</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Riepilogo rendicontato</t>
+  </si>
+  <si>
+    <t>Periodo I</t>
+  </si>
+  <si>
+    <t>Periodo II</t>
+  </si>
+  <si>
+    <t>Periodo III</t>
+  </si>
+  <si>
+    <t>totale</t>
   </si>
 </sst>
 </file>
@@ -5733,35 +5745,6 @@
                   <c:y val="-4.6153846153846247E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="0">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="ctr">
-                    <a:defRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="95000"/>
-                          <a:lumOff val="5000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="it-IT"/>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -5770,17 +5753,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:prstGeom prst="wedgeRectCallout">
-                      <a:avLst/>
-                    </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                  </c15:spPr>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-E02C-4DA9-9ACF-77FDA80CF46D}"/>
                 </c:ext>
@@ -14921,19 +14894,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S153"/>
+  <dimension ref="A1:AP153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="Q124" sqref="Q124"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AG45" sqref="AG45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="11" max="11" width="25.85546875" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
@@ -14944,7 +14921,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -14973,7 +14950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -15010,7 +14987,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -15047,7 +15024,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -15084,7 +15061,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -15121,7 +15098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -15158,7 +15135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -15195,7 +15172,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -15233,7 +15210,7 @@
         <v>4530</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -15266,7 +15243,263 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>18</v>
+      </c>
+      <c r="S13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="S14">
+        <f>R14*30</f>
+        <v>120</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC14">
+        <v>2</v>
+      </c>
+      <c r="AD14">
+        <f>AC14*30</f>
+        <v>60</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK14">
+        <v>6</v>
+      </c>
+      <c r="AL14">
+        <f>AK14*30</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Q15" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15">
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <f>R15*20</f>
+        <v>160</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC15">
+        <v>12</v>
+      </c>
+      <c r="AD15">
+        <f>AC15*20</f>
+        <v>240</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK15">
+        <v>10</v>
+      </c>
+      <c r="AL15">
+        <f>AK15*20</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>19</v>
+      </c>
+      <c r="S16">
+        <f>R16*25</f>
+        <v>475</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC16">
+        <v>20</v>
+      </c>
+      <c r="AD16">
+        <f>AC16*25</f>
+        <v>500</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK16">
+        <v>4</v>
+      </c>
+      <c r="AL16">
+        <f>AK16*25</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>11</v>
+      </c>
+      <c r="R17">
+        <v>24</v>
+      </c>
+      <c r="S17">
+        <f>R17*22</f>
+        <v>528</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC17">
+        <v>24</v>
+      </c>
+      <c r="AD17">
+        <f>AC17*22</f>
+        <v>528</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK17">
+        <v>12</v>
+      </c>
+      <c r="AL17">
+        <f>AK17*22</f>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R18">
+        <v>4</v>
+      </c>
+      <c r="S18">
+        <f>R18*15</f>
+        <v>60</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC18">
+        <v>14</v>
+      </c>
+      <c r="AD18">
+        <f>AC18*15</f>
+        <v>210</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK18">
+        <v>16</v>
+      </c>
+      <c r="AL18">
+        <f>AK18*15</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>13</v>
+      </c>
+      <c r="R19">
+        <v>27</v>
+      </c>
+      <c r="S19">
+        <f>R19*15</f>
+        <v>405</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19">
+        <v>9</v>
+      </c>
+      <c r="AD19">
+        <f>AC19*15</f>
+        <v>135</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK19">
+        <v>9</v>
+      </c>
+      <c r="AL19">
+        <f>AK19*15</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R20">
+        <f>SUM(R14:R19)</f>
+        <v>86</v>
+      </c>
+      <c r="S20">
+        <f>SUM(S14:S19)</f>
+        <v>1748</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC20">
+        <f>SUM(AC14:AC19)</f>
+        <v>81</v>
+      </c>
+      <c r="AD20">
+        <f>SUM(AD14:AD19)</f>
+        <v>1673</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK20">
+        <f>SUM(AK14:AK19)</f>
+        <v>57</v>
+      </c>
+      <c r="AL20">
+        <f>SUM(AL14:AL19)</f>
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC24">
+        <f>S20+AD20+AL20</f>
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>16</v>
       </c>
@@ -15276,8 +15509,35 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
+      <c r="R28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="AA28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AJ28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="3"/>
+      <c r="AO28" s="3"/>
+      <c r="AP28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>8</v>
       </c>
@@ -15305,8 +15565,71 @@
       <c r="M29" t="s">
         <v>19</v>
       </c>
+      <c r="R29" t="s">
+        <v>8</v>
+      </c>
+      <c r="S29" t="s">
+        <v>9</v>
+      </c>
+      <c r="T29" t="s">
+        <v>10</v>
+      </c>
+      <c r="U29" t="s">
+        <v>11</v>
+      </c>
+      <c r="V29" t="s">
+        <v>12</v>
+      </c>
+      <c r="W29" t="s">
+        <v>13</v>
+      </c>
+      <c r="X29" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN29" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -15342,8 +15665,83 @@
         <f>L30*30</f>
         <v>360</v>
       </c>
+      <c r="Q30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>4</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>4</v>
+      </c>
+      <c r="X30">
+        <f>SUM(R30:W30)</f>
+        <v>12</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <v>4</v>
+      </c>
+      <c r="AC30">
+        <v>3</v>
+      </c>
+      <c r="AD30">
+        <v>5</v>
+      </c>
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" ref="AG30:AG36" si="2">SUM(AA30:AF30)</f>
+        <v>12</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <v>3</v>
+      </c>
+      <c r="AL30">
+        <v>2</v>
+      </c>
+      <c r="AM30">
+        <v>0</v>
+      </c>
+      <c r="AN30">
+        <v>3</v>
+      </c>
+      <c r="AO30">
+        <v>0</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" ref="AP30:AP36" si="3">SUM(AJ30:AO30)</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -15366,7 +15764,7 @@
         <v>9</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H36" si="2">SUM(B31:G31)</f>
+        <f t="shared" ref="H31:H36" si="4">SUM(B31:G31)</f>
         <v>32</v>
       </c>
       <c r="K31" t="s">
@@ -15379,8 +15777,83 @@
         <f>L31*20</f>
         <v>600</v>
       </c>
+      <c r="Q31" t="s">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>4</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>5</v>
+      </c>
+      <c r="U31">
+        <v>3</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <f t="shared" ref="X31:X36" si="5">SUM(R31:W31)</f>
+        <v>12</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA31">
+        <v>2</v>
+      </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>0</v>
+      </c>
+      <c r="AE31">
+        <v>5</v>
+      </c>
+      <c r="AF31">
+        <v>4</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+      <c r="AM31">
+        <v>4</v>
+      </c>
+      <c r="AN31">
+        <v>0</v>
+      </c>
+      <c r="AO31">
+        <v>5</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -15403,7 +15876,7 @@
         <v>7</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K32" t="s">
@@ -15416,8 +15889,83 @@
         <f>L32*25</f>
         <v>1075</v>
       </c>
+      <c r="Q32" t="s">
+        <v>4</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>5</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>5</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32">
+        <v>6</v>
+      </c>
+      <c r="AD32">
+        <v>2</v>
+      </c>
+      <c r="AE32">
+        <v>2</v>
+      </c>
+      <c r="AF32">
+        <v>2</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <v>6</v>
+      </c>
+      <c r="AN32">
+        <v>4</v>
+      </c>
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -15440,7 +15988,7 @@
         <v>10</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K33" t="s">
@@ -15453,8 +16001,83 @@
         <f>L33*22</f>
         <v>1320</v>
       </c>
+      <c r="Q33" t="s">
+        <v>5</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>2</v>
+      </c>
+      <c r="U33">
+        <v>5</v>
+      </c>
+      <c r="V33">
+        <v>4</v>
+      </c>
+      <c r="W33">
+        <v>3</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <v>0</v>
+      </c>
+      <c r="AC33">
+        <v>3</v>
+      </c>
+      <c r="AD33">
+        <v>2</v>
+      </c>
+      <c r="AE33">
+        <v>1</v>
+      </c>
+      <c r="AF33">
+        <v>3</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+      <c r="AM33">
+        <v>2</v>
+      </c>
+      <c r="AN33">
+        <v>3</v>
+      </c>
+      <c r="AO33">
+        <v>4</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -15477,7 +16100,7 @@
         <v>5</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K34" t="s">
@@ -15490,8 +16113,83 @@
         <f>L34*15</f>
         <v>510</v>
       </c>
+      <c r="Q34" t="s">
+        <v>3</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>3</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>4</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>5</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <v>5</v>
+      </c>
+      <c r="AC34">
+        <v>3</v>
+      </c>
+      <c r="AD34">
+        <v>5</v>
+      </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>1</v>
+      </c>
+      <c r="AL34">
+        <v>2</v>
+      </c>
+      <c r="AM34">
+        <v>0</v>
+      </c>
+      <c r="AN34">
+        <v>4</v>
+      </c>
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -15514,7 +16212,7 @@
         <v>6</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K35" t="s">
@@ -15527,8 +16225,83 @@
         <f>L35*15</f>
         <v>675</v>
       </c>
+      <c r="Q35" t="s">
+        <v>2</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>3</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>5</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>6</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <v>3</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <v>3</v>
+      </c>
+      <c r="AE35">
+        <v>6</v>
+      </c>
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ35">
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <v>6</v>
+      </c>
+      <c r="AL35">
+        <v>0</v>
+      </c>
+      <c r="AM35">
+        <v>0</v>
+      </c>
+      <c r="AN35">
+        <v>0</v>
+      </c>
+      <c r="AO35">
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -15551,7 +16324,7 @@
         <v>4</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K36" s="1" t="s">
@@ -15565,8 +16338,83 @@
         <f>SUM(M30:M35)</f>
         <v>4540</v>
       </c>
+      <c r="Q36" t="s">
+        <v>17</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>5</v>
+      </c>
+      <c r="U36">
+        <v>3</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>4</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <v>5</v>
+      </c>
+      <c r="AD36">
+        <v>7</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ36">
+        <v>6</v>
+      </c>
+      <c r="AK36">
+        <v>0</v>
+      </c>
+      <c r="AL36">
+        <v>0</v>
+      </c>
+      <c r="AM36">
+        <v>0</v>
+      </c>
+      <c r="AN36">
+        <v>2</v>
+      </c>
+      <c r="AO36">
+        <v>0</v>
+      </c>
+      <c r="AP36">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -15575,28 +16423,121 @@
         <v>12</v>
       </c>
       <c r="C37">
-        <f t="shared" ref="C37" si="3">SUM(C30:C36)</f>
+        <f t="shared" ref="C37" si="6">SUM(C30:C36)</f>
         <v>30</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37" si="4">SUM(D30:D36)</f>
+        <f t="shared" ref="D37" si="7">SUM(D30:D36)</f>
         <v>43</v>
       </c>
       <c r="E37">
-        <f t="shared" ref="E37" si="5">SUM(E30:E36)</f>
+        <f t="shared" ref="E37" si="8">SUM(E30:E36)</f>
         <v>60</v>
       </c>
       <c r="F37">
-        <f t="shared" ref="F37" si="6">SUM(F30:F36)</f>
+        <f t="shared" ref="F37" si="9">SUM(F30:F36)</f>
         <v>34</v>
       </c>
       <c r="G37">
-        <f t="shared" ref="G37" si="7">SUM(G30:G36)</f>
+        <f t="shared" ref="G37" si="10">SUM(G30:G36)</f>
         <v>45</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37" si="8">SUM(H30:H36)</f>
+        <f t="shared" ref="H37" si="11">SUM(H30:H36)</f>
         <v>224</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R37">
+        <f>SUM(R30:R36)</f>
+        <v>4</v>
+      </c>
+      <c r="S37">
+        <f t="shared" ref="S37:X37" si="12">SUM(S30:S36)</f>
+        <v>8</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="12"/>
+        <v>19</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="12"/>
+        <v>27</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="12"/>
+        <v>86</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" ref="AA37:AG37" si="13">SUM(AA30:AA36)</f>
+        <v>2</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="13"/>
+        <v>12</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="13"/>
+        <v>81</v>
+      </c>
+      <c r="AI37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ37">
+        <f t="shared" ref="AJ37:AP37" si="14">SUM(AJ30:AJ36)</f>
+        <v>6</v>
+      </c>
+      <c r="AK37">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="AL37">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="AM37">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="AN37">
+        <f t="shared" si="14"/>
+        <v>16</v>
+      </c>
+      <c r="AO37">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="AP37">
+        <f t="shared" si="14"/>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -15662,7 +16603,7 @@
         <v>13</v>
       </c>
       <c r="H57">
-        <f t="shared" ref="H57:H63" si="9">SUM(B57:G57)</f>
+        <f t="shared" ref="H57:H63" si="15">SUM(B57:G57)</f>
         <v>50</v>
       </c>
       <c r="K57" t="s">
@@ -15699,7 +16640,7 @@
         <v>15</v>
       </c>
       <c r="H58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>50</v>
       </c>
       <c r="K58" t="s">
@@ -15736,7 +16677,7 @@
         <v>10</v>
       </c>
       <c r="H59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>50</v>
       </c>
       <c r="K59" t="s">
@@ -15773,7 +16714,7 @@
         <v>12</v>
       </c>
       <c r="H60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>50</v>
       </c>
       <c r="K60" t="s">
@@ -15810,7 +16751,7 @@
         <v>10</v>
       </c>
       <c r="H61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>50</v>
       </c>
       <c r="K61" t="s">
@@ -15847,7 +16788,7 @@
         <v>11</v>
       </c>
       <c r="H62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>50</v>
       </c>
       <c r="K62" t="s">
@@ -15884,7 +16825,7 @@
         <v>10</v>
       </c>
       <c r="H63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>50</v>
       </c>
       <c r="K63" s="1" t="s">
@@ -15908,27 +16849,27 @@
         <v>20</v>
       </c>
       <c r="C64">
-        <f t="shared" ref="C64" si="10">SUM(C57:C63)</f>
+        <f t="shared" ref="C64" si="16">SUM(C57:C63)</f>
         <v>27</v>
       </c>
       <c r="D64">
-        <f t="shared" ref="D64" si="11">SUM(D57:D63)</f>
+        <f t="shared" ref="D64" si="17">SUM(D57:D63)</f>
         <v>0</v>
       </c>
       <c r="E64">
-        <f t="shared" ref="E64" si="12">SUM(E57:E63)</f>
+        <f t="shared" ref="E64" si="18">SUM(E57:E63)</f>
         <v>75</v>
       </c>
       <c r="F64">
-        <f t="shared" ref="F64" si="13">SUM(F57:F63)</f>
+        <f t="shared" ref="F64" si="19">SUM(F57:F63)</f>
         <v>147</v>
       </c>
       <c r="G64">
-        <f t="shared" ref="G64" si="14">SUM(G57:G63)</f>
+        <f t="shared" ref="G64" si="20">SUM(G57:G63)</f>
         <v>81</v>
       </c>
       <c r="H64">
-        <f t="shared" ref="H64" si="15">SUM(H57:H63)</f>
+        <f t="shared" ref="H64" si="21">SUM(H57:H63)</f>
         <v>350</v>
       </c>
     </row>
@@ -15995,7 +16936,7 @@
         <v>11</v>
       </c>
       <c r="H82">
-        <f t="shared" ref="H82:H88" si="16">SUM(B82:G82)</f>
+        <f t="shared" ref="H82:H88" si="22">SUM(B82:G82)</f>
         <v>20</v>
       </c>
       <c r="K82" t="s">
@@ -16032,7 +16973,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="K83" t="s">
@@ -16069,7 +17010,7 @@
         <v>6</v>
       </c>
       <c r="H84">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="K84" t="s">
@@ -16106,7 +17047,7 @@
         <v>5</v>
       </c>
       <c r="H85">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="K85" t="s">
@@ -16143,7 +17084,7 @@
         <v>11</v>
       </c>
       <c r="H86">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="K86" t="s">
@@ -16180,7 +17121,7 @@
         <v>12</v>
       </c>
       <c r="H87">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="K87" t="s">
@@ -16217,7 +17158,7 @@
         <v>10</v>
       </c>
       <c r="H88">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="K88" s="1" t="s">
@@ -16241,27 +17182,27 @@
         <v>20</v>
       </c>
       <c r="C89">
-        <f t="shared" ref="C89" si="17">SUM(C82:C88)</f>
+        <f t="shared" ref="C89" si="23">SUM(C82:C88)</f>
         <v>20</v>
       </c>
       <c r="D89">
-        <f t="shared" ref="D89" si="18">SUM(D82:D88)</f>
+        <f t="shared" ref="D89" si="24">SUM(D82:D88)</f>
         <v>0</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89" si="19">SUM(E82:E88)</f>
+        <f t="shared" ref="E89" si="25">SUM(E82:E88)</f>
         <v>15</v>
       </c>
       <c r="F89">
-        <f t="shared" ref="F89" si="20">SUM(F82:F88)</f>
+        <f t="shared" ref="F89" si="26">SUM(F82:F88)</f>
         <v>30</v>
       </c>
       <c r="G89">
-        <f t="shared" ref="G89" si="21">SUM(G82:G88)</f>
+        <f t="shared" ref="G89" si="27">SUM(G82:G88)</f>
         <v>55</v>
       </c>
       <c r="H89">
-        <f t="shared" ref="H89" si="22">SUM(H82:H88)</f>
+        <f t="shared" ref="H89" si="28">SUM(H82:H88)</f>
         <v>140</v>
       </c>
     </row>
@@ -16314,27 +17255,27 @@
         <v>14</v>
       </c>
       <c r="C109">
-        <f t="shared" ref="C109:H109" si="23">SUM(C3,C30,C57,C82)</f>
+        <f t="shared" ref="C109:H109" si="29">SUM(C3,C30,C57,C82)</f>
         <v>19</v>
       </c>
       <c r="D109">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>19</v>
       </c>
       <c r="E109">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="F109">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>28</v>
       </c>
       <c r="G109">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>32</v>
       </c>
       <c r="H109">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>132</v>
       </c>
       <c r="K109" t="s">
@@ -16354,38 +17295,38 @@
         <v>1</v>
       </c>
       <c r="B110">
-        <f t="shared" ref="B110:H116" si="24">SUM(B4,B31,B58,B83)</f>
+        <f t="shared" ref="B110:H116" si="30">SUM(B4,B31,B58,B83)</f>
         <v>12</v>
       </c>
       <c r="C110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>22</v>
       </c>
       <c r="D110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>7</v>
       </c>
       <c r="E110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>23</v>
       </c>
       <c r="F110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>30</v>
       </c>
       <c r="G110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>38</v>
       </c>
       <c r="H110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>132</v>
       </c>
       <c r="K110" t="s">
         <v>9</v>
       </c>
       <c r="L110">
-        <f t="shared" ref="L110:L115" si="25">SUM(L4,L31,L58,L83)</f>
+        <f t="shared" ref="L110:L115" si="31">SUM(L4,L31,L58,L83)</f>
         <v>122</v>
       </c>
       <c r="M110">
@@ -16398,38 +17339,38 @@
         <v>4</v>
       </c>
       <c r="B111">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>14</v>
       </c>
       <c r="C111">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
       <c r="D111">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>15</v>
       </c>
       <c r="E111">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>23</v>
       </c>
       <c r="F111">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>27</v>
       </c>
       <c r="G111">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>37</v>
       </c>
       <c r="H111">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>132</v>
       </c>
       <c r="K111" t="s">
         <v>10</v>
       </c>
       <c r="L111">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>121</v>
       </c>
       <c r="M111">
@@ -16442,38 +17383,38 @@
         <v>5</v>
       </c>
       <c r="B112">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>6</v>
       </c>
       <c r="C112">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>13</v>
       </c>
       <c r="D112">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>22</v>
       </c>
       <c r="E112">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>22</v>
       </c>
       <c r="F112">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>36</v>
       </c>
       <c r="G112">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>33</v>
       </c>
       <c r="H112">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>132</v>
       </c>
       <c r="K112" t="s">
         <v>11</v>
       </c>
       <c r="L112">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>150</v>
       </c>
       <c r="M112">
@@ -16486,38 +17427,38 @@
         <v>3</v>
       </c>
       <c r="B113">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>11</v>
       </c>
       <c r="C113">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>15</v>
       </c>
       <c r="D113">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>18</v>
       </c>
       <c r="E113">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>22</v>
       </c>
       <c r="F113">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>34</v>
       </c>
       <c r="G113">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>32</v>
       </c>
       <c r="H113">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>132</v>
       </c>
       <c r="K113" t="s">
         <v>12</v>
       </c>
       <c r="L113">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>211</v>
       </c>
       <c r="M113">
@@ -16530,38 +17471,38 @@
         <v>2</v>
       </c>
       <c r="B114">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
       <c r="C114">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>17</v>
       </c>
       <c r="D114">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>22</v>
       </c>
       <c r="E114">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>21</v>
       </c>
       <c r="F114">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>27</v>
       </c>
       <c r="G114">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>37</v>
       </c>
       <c r="H114">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>132</v>
       </c>
       <c r="K114" t="s">
         <v>13</v>
       </c>
       <c r="L114">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>243</v>
       </c>
       <c r="M114">
@@ -16574,38 +17515,38 @@
         <v>17</v>
       </c>
       <c r="B115">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="C115">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>20</v>
       </c>
       <c r="D115">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>18</v>
       </c>
       <c r="E115">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>19</v>
       </c>
       <c r="F115">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>29</v>
       </c>
       <c r="G115">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>34</v>
       </c>
       <c r="H115">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>132</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L115">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>924</v>
       </c>
       <c r="M115">
@@ -16618,31 +17559,31 @@
         <v>7</v>
       </c>
       <c r="B116">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>77</v>
       </c>
       <c r="C116">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>122</v>
       </c>
       <c r="D116">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>121</v>
       </c>
       <c r="E116">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>150</v>
       </c>
       <c r="F116">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>211</v>
       </c>
       <c r="G116">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>243</v>
       </c>
       <c r="H116">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>924</v>
       </c>
     </row>
@@ -16701,27 +17642,27 @@
         <v>0</v>
       </c>
       <c r="C137">
-        <f t="shared" ref="C137:H137" si="26">SUM(C82,C57,C30)</f>
+        <f t="shared" ref="C137:H137" si="32">SUM(C82,C57,C30)</f>
         <v>19</v>
       </c>
       <c r="D137">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>7</v>
       </c>
       <c r="E137">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>20</v>
       </c>
       <c r="F137">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>28</v>
       </c>
       <c r="G137">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>28</v>
       </c>
       <c r="H137">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>102</v>
       </c>
       <c r="K137" t="s">
@@ -16741,38 +17682,38 @@
         <v>1</v>
       </c>
       <c r="B138">
-        <f t="shared" ref="B138:H144" si="27">SUM(B83,B58,B31)</f>
+        <f t="shared" ref="B138:H144" si="33">SUM(B83,B58,B31)</f>
         <v>12</v>
       </c>
       <c r="C138">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>8</v>
       </c>
       <c r="D138">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="E138">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>23</v>
       </c>
       <c r="F138">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="G138">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>24</v>
       </c>
       <c r="H138">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>102</v>
       </c>
       <c r="K138" t="s">
         <v>9</v>
       </c>
       <c r="L138">
-        <f t="shared" ref="L138:L143" si="28">SUM(L83,L58,L31)</f>
+        <f t="shared" ref="L138:L143" si="34">SUM(L83,L58,L31)</f>
         <v>77</v>
       </c>
       <c r="M138">
@@ -16785,38 +17726,38 @@
         <v>4</v>
       </c>
       <c r="B139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>14</v>
       </c>
       <c r="C139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>4</v>
       </c>
       <c r="D139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>11</v>
       </c>
       <c r="E139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>23</v>
       </c>
       <c r="F139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>27</v>
       </c>
       <c r="G139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>23</v>
       </c>
       <c r="H139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>102</v>
       </c>
       <c r="K139" t="s">
         <v>10</v>
       </c>
       <c r="L139">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>43</v>
       </c>
       <c r="M139">
@@ -16829,38 +17770,38 @@
         <v>5</v>
       </c>
       <c r="B140">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="C140">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="D140">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="E140">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>22</v>
       </c>
       <c r="F140">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>36</v>
       </c>
       <c r="G140">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>27</v>
       </c>
       <c r="H140">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>102</v>
       </c>
       <c r="K140" t="s">
         <v>11</v>
       </c>
       <c r="L140">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>150</v>
       </c>
       <c r="M140">
@@ -16873,38 +17814,38 @@
         <v>3</v>
       </c>
       <c r="B141">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="C141">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>15</v>
       </c>
       <c r="D141">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="E141">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>22</v>
       </c>
       <c r="F141">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>34</v>
       </c>
       <c r="G141">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>26</v>
       </c>
       <c r="H141">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>102</v>
       </c>
       <c r="K141" t="s">
         <v>12</v>
       </c>
       <c r="L141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>211</v>
       </c>
       <c r="M141">
@@ -16917,38 +17858,38 @@
         <v>2</v>
       </c>
       <c r="B142">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>8</v>
       </c>
       <c r="C142">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>17</v>
       </c>
       <c r="D142">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="E142">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>21</v>
       </c>
       <c r="F142">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>27</v>
       </c>
       <c r="G142">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>29</v>
       </c>
       <c r="H142">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>102</v>
       </c>
       <c r="K142" t="s">
         <v>13</v>
       </c>
       <c r="L142">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>181</v>
       </c>
       <c r="M142">
@@ -16961,38 +17902,38 @@
         <v>17</v>
       </c>
       <c r="B143">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>12</v>
       </c>
       <c r="C143">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>8</v>
       </c>
       <c r="D143">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="E143">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>19</v>
       </c>
       <c r="F143">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>29</v>
       </c>
       <c r="G143">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>24</v>
       </c>
       <c r="H143">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>102</v>
       </c>
       <c r="K143" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L143">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>714</v>
       </c>
       <c r="M143">
@@ -17005,31 +17946,31 @@
         <v>7</v>
       </c>
       <c r="B144">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>52</v>
       </c>
       <c r="C144">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>77</v>
       </c>
       <c r="D144">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>43</v>
       </c>
       <c r="E144">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>150</v>
       </c>
       <c r="F144">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>211</v>
       </c>
       <c r="G144">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>181</v>
       </c>
       <c r="H144">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>714</v>
       </c>
     </row>
@@ -17037,7 +17978,10 @@
       <c r="S153" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="R28:X28"/>
+    <mergeCell ref="AA28:AG28"/>
+    <mergeCell ref="AJ28:AP28"/>
     <mergeCell ref="B135:H135"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B28:H28"/>

</xml_diff>

<commit_message>
fix preventivo prog arch
</commit_message>
<xml_diff>
--- a/DocEsterna/PianoDiProgetto/Charts/GraficiPreventivo.xlsx
+++ b/DocEsterna/PianoDiProgetto/Charts/GraficiPreventivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SWE\RepoDocumentazione\CodeBusters-Docs\DocEsterna\PianoDiProgetto\Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1945A6C-D092-4A7B-A5C4-97D303088366}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C4641C-9C53-4CEF-9E5F-3248754F79E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="35">
   <si>
     <t>Baldisseri Michele</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>totale</t>
-  </si>
-  <si>
-    <t>I</t>
   </si>
   <si>
     <t>II</t>
@@ -196,11 +193,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2727,6 +2724,9 @@
                 <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2796,6 +2796,9 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -3020,7 +3023,13 @@
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
                 <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -3091,23 +3100,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3198,25 +3210,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3504,8 +3516,11 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3577,6 +3592,12 @@
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3721,13 +3742,16 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3797,14 +3821,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3874,8 +3910,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3966,25 +4014,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31498,8 +31546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DI153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AN98" sqref="AN98"/>
+    <sheetView tabSelected="1" topLeftCell="Q51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W57" sqref="W57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31514,15 +31562,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -32103,42 +32151,42 @@
       </c>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="R28" s="4" t="s">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="R28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="AA28" s="4" t="s">
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="AA28" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
-      <c r="AG28" s="4"/>
-      <c r="AJ28" s="4" t="s">
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="6"/>
+      <c r="AG28" s="6"/>
+      <c r="AJ28" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AK28" s="4"/>
-      <c r="AL28" s="4"/>
-      <c r="AM28" s="4"/>
-      <c r="AN28" s="4"/>
-      <c r="AO28" s="4"/>
-      <c r="AP28" s="4"/>
+      <c r="AK28" s="6"/>
+      <c r="AL28" s="6"/>
+      <c r="AM28" s="6"/>
+      <c r="AN28" s="6"/>
+      <c r="AO28" s="6"/>
+      <c r="AP28" s="6"/>
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -32868,7 +32916,7 @@
       <c r="AD35">
         <v>3</v>
       </c>
-      <c r="AE35" s="5">
+      <c r="AE35" s="4">
         <v>6</v>
       </c>
       <c r="AF35">
@@ -33143,7 +33191,23 @@
         <v>57</v>
       </c>
     </row>
+    <row r="41" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="AX41" s="3"/>
+      <c r="AY41" s="3"/>
+      <c r="AZ41" s="3"/>
+      <c r="BA41" s="3"/>
+      <c r="BB41" s="3"/>
+      <c r="BC41" s="3"/>
+      <c r="BD41" s="3"/>
+    </row>
     <row r="42" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="AS42" s="3"/>
+      <c r="AT42" s="3"/>
+      <c r="AU42" s="3"/>
+      <c r="AV42" s="3"/>
+      <c r="AW42" s="3"/>
+      <c r="AX42" s="3"/>
+      <c r="AY42" s="3"/>
       <c r="CG42" s="3"/>
       <c r="CH42" s="3"/>
       <c r="CI42" s="3"/>
@@ -33153,78 +33217,78 @@
       <c r="CM42" s="3"/>
     </row>
     <row r="55" spans="1:113" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="R55" s="4" t="s">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="R55" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+      <c r="U55" s="6"/>
+      <c r="V55" s="6"/>
+      <c r="W55" s="6"/>
+      <c r="X55" s="6"/>
+      <c r="AF55" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
-      <c r="X55" s="4"/>
-      <c r="AF55" s="4" t="s">
+      <c r="AG55" s="6"/>
+      <c r="AH55" s="6"/>
+      <c r="AI55" s="6"/>
+      <c r="AJ55" s="6"/>
+      <c r="AK55" s="6"/>
+      <c r="AL55" s="6"/>
+      <c r="AT55" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AG55" s="4"/>
-      <c r="AH55" s="4"/>
-      <c r="AI55" s="4"/>
-      <c r="AJ55" s="4"/>
-      <c r="AK55" s="4"/>
-      <c r="AL55" s="4"/>
-      <c r="AT55" s="4" t="s">
+      <c r="AU55" s="6"/>
+      <c r="AV55" s="6"/>
+      <c r="AW55" s="6"/>
+      <c r="AX55" s="6"/>
+      <c r="AY55" s="6"/>
+      <c r="AZ55" s="6"/>
+      <c r="BH55" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AU55" s="4"/>
-      <c r="AV55" s="4"/>
-      <c r="AW55" s="4"/>
-      <c r="AX55" s="4"/>
-      <c r="AY55" s="4"/>
-      <c r="AZ55" s="4"/>
-      <c r="BH55" s="4" t="s">
+      <c r="BI55" s="6"/>
+      <c r="BJ55" s="6"/>
+      <c r="BK55" s="6"/>
+      <c r="BL55" s="6"/>
+      <c r="BM55" s="6"/>
+      <c r="BN55" s="6"/>
+      <c r="BV55" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="BI55" s="4"/>
-      <c r="BJ55" s="4"/>
-      <c r="BK55" s="4"/>
-      <c r="BL55" s="4"/>
-      <c r="BM55" s="4"/>
-      <c r="BN55" s="4"/>
-      <c r="BV55" s="4" t="s">
+      <c r="BW55" s="6"/>
+      <c r="BX55" s="6"/>
+      <c r="BY55" s="6"/>
+      <c r="BZ55" s="6"/>
+      <c r="CA55" s="6"/>
+      <c r="CB55" s="6"/>
+      <c r="CJ55" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="BW55" s="4"/>
-      <c r="BX55" s="4"/>
-      <c r="BY55" s="4"/>
-      <c r="BZ55" s="4"/>
-      <c r="CA55" s="4"/>
-      <c r="CB55" s="4"/>
-      <c r="CJ55" s="4" t="s">
+      <c r="CK55" s="6"/>
+      <c r="CL55" s="6"/>
+      <c r="CM55" s="6"/>
+      <c r="CN55" s="6"/>
+      <c r="CO55" s="6"/>
+      <c r="CP55" s="6"/>
+      <c r="CX55" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="CK55" s="4"/>
-      <c r="CL55" s="4"/>
-      <c r="CM55" s="4"/>
-      <c r="CN55" s="4"/>
-      <c r="CO55" s="4"/>
-      <c r="CP55" s="4"/>
-      <c r="CX55" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="CY55" s="4"/>
-      <c r="CZ55" s="4"/>
-      <c r="DA55" s="4"/>
-      <c r="DB55" s="4"/>
-      <c r="DC55" s="4"/>
-      <c r="DD55" s="4"/>
+      <c r="CY55" s="6"/>
+      <c r="CZ55" s="6"/>
+      <c r="DA55" s="6"/>
+      <c r="DB55" s="6"/>
+      <c r="DC55" s="6"/>
+      <c r="DD55" s="6"/>
     </row>
     <row r="56" spans="1:113" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -33489,20 +33553,24 @@
       <c r="U57">
         <v>2</v>
       </c>
+      <c r="W57">
+        <v>6</v>
+      </c>
       <c r="X57">
         <f t="shared" ref="X57:X63" si="16">SUM(R57:W57)</f>
-        <v>4</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="Z57" s="2"/>
       <c r="AA57" t="s">
         <v>8</v>
       </c>
       <c r="AB57">
         <f>SUM(R57:R63)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC57">
         <f>AB57*30</f>
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="AE57" t="s">
         <v>0</v>
@@ -33513,20 +33581,26 @@
       <c r="AI57">
         <v>4</v>
       </c>
+      <c r="AJ57">
+        <v>2</v>
+      </c>
+      <c r="AK57">
+        <v>4</v>
+      </c>
       <c r="AL57">
         <f t="shared" ref="AL57:AL63" si="17">SUM(AF57:AK57)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AO57" t="s">
         <v>8</v>
       </c>
       <c r="AP57">
         <f>SUM(AF57:AF63)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AQ57">
         <f>AP57*30</f>
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="AS57" t="s">
         <v>0</v>
@@ -33686,22 +33760,22 @@
         <v>2</v>
       </c>
       <c r="W58">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="X58">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="AA58" t="s">
         <v>9</v>
       </c>
       <c r="AB58">
         <f>SUM(S57:S63)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC58">
         <f>AB58*20</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="AE58" t="s">
         <v>1</v>
@@ -33710,22 +33784,25 @@
         <v>5</v>
       </c>
       <c r="AJ58">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="AK58">
+        <v>4</v>
       </c>
       <c r="AL58">
         <f t="shared" si="17"/>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="AO58" t="s">
         <v>9</v>
       </c>
       <c r="AP58">
         <f>SUM(AG57:AG63)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AQ58">
         <f>AP58*20</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="AS58" t="s">
         <v>1</v>
@@ -33890,12 +33967,15 @@
       <c r="U59">
         <v>3</v>
       </c>
+      <c r="V59">
+        <v>4</v>
+      </c>
       <c r="W59">
         <v>2</v>
       </c>
       <c r="X59">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AA59" t="s">
         <v>10</v>
@@ -33912,14 +33992,17 @@
         <v>4</v>
       </c>
       <c r="AI59">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="AJ59">
+        <v>7</v>
       </c>
       <c r="AK59">
         <v>3</v>
       </c>
       <c r="AL59">
         <f t="shared" si="17"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="AO59" t="s">
         <v>10</v>
@@ -34090,17 +34173,17 @@
         <v>1650</v>
       </c>
       <c r="Q60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U60">
         <v>1</v>
       </c>
       <c r="W60">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="X60">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AA60" t="s">
         <v>11</v>
@@ -34114,28 +34197,34 @@
         <v>220</v>
       </c>
       <c r="AE60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI60">
         <v>6</v>
       </c>
+      <c r="AJ60">
+        <v>8</v>
+      </c>
+      <c r="AK60">
+        <v>2</v>
+      </c>
       <c r="AL60">
         <f t="shared" si="17"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="AO60" t="s">
         <v>11</v>
       </c>
       <c r="AP60">
         <f>SUM(AI57:AI63)</f>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AQ60">
         <f>AP60*22</f>
-        <v>484</v>
+        <v>594</v>
       </c>
       <c r="AS60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AT60">
         <v>2</v>
@@ -34162,7 +34251,7 @@
         <v>506</v>
       </c>
       <c r="BG60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BH60">
         <v>2</v>
@@ -34189,7 +34278,7 @@
         <v>242</v>
       </c>
       <c r="BU60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BV60">
         <v>2</v>
@@ -34216,7 +34305,7 @@
         <v>88</v>
       </c>
       <c r="CI60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="CN60">
         <v>6</v>
@@ -34240,7 +34329,7 @@
         <v>110</v>
       </c>
       <c r="CW60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="DB60">
         <v>2</v>
@@ -34307,46 +34396,55 @@
         <v>1</v>
       </c>
       <c r="V61">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W61">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="X61">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="AA61" t="s">
         <v>12</v>
       </c>
       <c r="AB61">
         <f>SUM(V57:V63)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="AC61">
         <f>AB61*15</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="AE61" t="s">
         <v>3</v>
       </c>
+      <c r="AG61">
+        <v>2</v>
+      </c>
       <c r="AI61">
         <v>5</v>
       </c>
+      <c r="AJ61">
+        <v>5</v>
+      </c>
+      <c r="AK61">
+        <v>2</v>
+      </c>
       <c r="AL61">
         <f t="shared" si="17"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="AO61" t="s">
         <v>12</v>
       </c>
       <c r="AP61">
         <f>SUM(AJ57:AJ63)</f>
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="AQ61">
         <f>AP61*15</f>
-        <v>195</v>
+        <v>765</v>
       </c>
       <c r="AS61" t="s">
         <v>3</v>
@@ -34511,44 +34609,56 @@
       <c r="R62">
         <v>2</v>
       </c>
+      <c r="S62">
+        <v>2</v>
+      </c>
+      <c r="V62">
+        <v>2</v>
+      </c>
       <c r="W62">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="X62">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="AA62" t="s">
         <v>13</v>
       </c>
       <c r="AB62">
         <f>SUM(W57:W63)</f>
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="AC62">
         <f>AB62*15</f>
-        <v>210</v>
+        <v>675</v>
       </c>
       <c r="AE62" t="s">
         <v>2</v>
       </c>
+      <c r="AF62">
+        <v>2</v>
+      </c>
+      <c r="AI62">
+        <v>2</v>
+      </c>
       <c r="AJ62">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AL62">
         <f t="shared" si="17"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="AO62" t="s">
         <v>13</v>
       </c>
       <c r="AP62">
         <f>SUM(AK57:AK63)</f>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AQ62">
         <f>AP62*15</f>
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="AS62" t="s">
         <v>2</v>
@@ -34720,50 +34830,56 @@
       <c r="Q63" t="s">
         <v>17</v>
       </c>
+      <c r="R63">
+        <v>3</v>
+      </c>
       <c r="U63">
         <v>3</v>
       </c>
       <c r="W63">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X63">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AA63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AB63">
         <f>SUM(AB57:AB62)</f>
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="AC63">
         <f>SUM(AC57:AC62)</f>
-        <v>590</v>
+        <v>1305</v>
       </c>
       <c r="AE63" t="s">
         <v>17</v>
       </c>
       <c r="AF63">
+        <v>2</v>
+      </c>
+      <c r="AG63">
         <v>1</v>
       </c>
       <c r="AJ63">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AL63">
         <f t="shared" si="17"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="AO63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AP63">
         <f>SUM(AP57:AP62)</f>
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="AQ63">
         <f>SUM(AQ57:AQ62)</f>
-        <v>814</v>
+        <v>1824</v>
       </c>
       <c r="AS63" t="s">
         <v>17</v>
@@ -34926,33 +35042,33 @@
       </c>
     </row>
     <row r="80" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="R80" s="4" t="s">
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="R80" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S80" s="6"/>
+      <c r="T80" s="6"/>
+      <c r="U80" s="6"/>
+      <c r="V80" s="6"/>
+      <c r="W80" s="6"/>
+      <c r="X80" s="6"/>
+      <c r="AF80" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S80" s="4"/>
-      <c r="T80" s="4"/>
-      <c r="U80" s="4"/>
-      <c r="V80" s="4"/>
-      <c r="W80" s="4"/>
-      <c r="X80" s="4"/>
-      <c r="AF80" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG80" s="4"/>
-      <c r="AH80" s="4"/>
-      <c r="AI80" s="4"/>
-      <c r="AJ80" s="4"/>
-      <c r="AK80" s="4"/>
-      <c r="AL80" s="4"/>
+      <c r="AG80" s="6"/>
+      <c r="AH80" s="6"/>
+      <c r="AI80" s="6"/>
+      <c r="AJ80" s="6"/>
+      <c r="AK80" s="6"/>
+      <c r="AL80" s="6"/>
     </row>
     <row r="81" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
@@ -35819,7 +35935,7 @@
       </c>
     </row>
     <row r="91" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Q91" s="6"/>
+      <c r="Q91" s="5"/>
       <c r="R91" s="3"/>
       <c r="S91" s="3"/>
       <c r="T91" s="3"/>
@@ -35829,7 +35945,7 @@
       <c r="X91" s="3"/>
     </row>
     <row r="92" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Q92" s="6"/>
+      <c r="Q92" s="5"/>
       <c r="R92" s="3"/>
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
@@ -35839,95 +35955,95 @@
       <c r="X92" s="3"/>
     </row>
     <row r="93" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Q93" s="6"/>
-      <c r="R93" s="6"/>
-      <c r="S93" s="6"/>
-      <c r="T93" s="6"/>
-      <c r="U93" s="6"/>
-      <c r="V93" s="6"/>
-      <c r="W93" s="6"/>
-      <c r="X93" s="6"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="5"/>
+      <c r="V93" s="5"/>
+      <c r="W93" s="5"/>
+      <c r="X93" s="5"/>
     </row>
     <row r="94" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Q94" s="6"/>
-      <c r="R94" s="6"/>
-      <c r="S94" s="6"/>
-      <c r="T94" s="6"/>
-      <c r="U94" s="6"/>
-      <c r="V94" s="6"/>
-      <c r="W94" s="6"/>
-      <c r="X94" s="6"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="5"/>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+      <c r="U94" s="5"/>
+      <c r="V94" s="5"/>
+      <c r="W94" s="5"/>
+      <c r="X94" s="5"/>
     </row>
     <row r="95" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Q95" s="6"/>
-      <c r="R95" s="6"/>
-      <c r="S95" s="6"/>
-      <c r="T95" s="6"/>
-      <c r="U95" s="6"/>
-      <c r="V95" s="6"/>
-      <c r="W95" s="6"/>
-      <c r="X95" s="6"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="5"/>
+      <c r="V95" s="5"/>
+      <c r="W95" s="5"/>
+      <c r="X95" s="5"/>
     </row>
     <row r="96" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Q96" s="6"/>
-      <c r="R96" s="6"/>
-      <c r="S96" s="6"/>
-      <c r="T96" s="6"/>
-      <c r="U96" s="6"/>
-      <c r="V96" s="6"/>
-      <c r="W96" s="6"/>
-      <c r="X96" s="6"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+      <c r="T96" s="5"/>
+      <c r="U96" s="5"/>
+      <c r="V96" s="5"/>
+      <c r="W96" s="5"/>
+      <c r="X96" s="5"/>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="Q97" s="6"/>
-      <c r="R97" s="6"/>
-      <c r="S97" s="6"/>
-      <c r="T97" s="6"/>
-      <c r="U97" s="6"/>
-      <c r="V97" s="6"/>
-      <c r="W97" s="6"/>
-      <c r="X97" s="6"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+      <c r="U97" s="5"/>
+      <c r="V97" s="5"/>
+      <c r="W97" s="5"/>
+      <c r="X97" s="5"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="Q98" s="6"/>
-      <c r="R98" s="6"/>
-      <c r="S98" s="6"/>
-      <c r="T98" s="6"/>
-      <c r="U98" s="6"/>
-      <c r="V98" s="6"/>
-      <c r="W98" s="6"/>
-      <c r="X98" s="6"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="5"/>
+      <c r="S98" s="5"/>
+      <c r="T98" s="5"/>
+      <c r="U98" s="5"/>
+      <c r="V98" s="5"/>
+      <c r="W98" s="5"/>
+      <c r="X98" s="5"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="Q99" s="6"/>
-      <c r="R99" s="6"/>
-      <c r="S99" s="6"/>
-      <c r="T99" s="6"/>
-      <c r="U99" s="6"/>
-      <c r="V99" s="6"/>
-      <c r="W99" s="6"/>
-      <c r="X99" s="6"/>
+      <c r="Q99" s="5"/>
+      <c r="R99" s="5"/>
+      <c r="S99" s="5"/>
+      <c r="T99" s="5"/>
+      <c r="U99" s="5"/>
+      <c r="V99" s="5"/>
+      <c r="W99" s="5"/>
+      <c r="X99" s="5"/>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="Q100" s="6"/>
-      <c r="R100" s="6"/>
-      <c r="S100" s="6"/>
-      <c r="T100" s="6"/>
-      <c r="U100" s="6"/>
-      <c r="V100" s="6"/>
-      <c r="W100" s="6"/>
-      <c r="X100" s="6"/>
+      <c r="Q100" s="5"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="5"/>
+      <c r="T100" s="5"/>
+      <c r="U100" s="5"/>
+      <c r="V100" s="5"/>
+      <c r="W100" s="5"/>
+      <c r="X100" s="5"/>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
@@ -36306,15 +36422,15 @@
       <c r="I134" s="2"/>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="4"/>
-      <c r="F135" s="4"/>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
@@ -36691,11 +36807,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AT55:AZ55"/>
-    <mergeCell ref="BH55:BN55"/>
-    <mergeCell ref="BV55:CB55"/>
-    <mergeCell ref="CJ55:CP55"/>
-    <mergeCell ref="CX55:DD55"/>
     <mergeCell ref="R28:X28"/>
     <mergeCell ref="AA28:AG28"/>
     <mergeCell ref="AJ28:AP28"/>
@@ -36709,6 +36820,11 @@
     <mergeCell ref="AF55:AL55"/>
     <mergeCell ref="R80:X80"/>
     <mergeCell ref="AF80:AL80"/>
+    <mergeCell ref="AT55:AZ55"/>
+    <mergeCell ref="BH55:BN55"/>
+    <mergeCell ref="BV55:CB55"/>
+    <mergeCell ref="CJ55:CP55"/>
+    <mergeCell ref="CX55:DD55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>